<commit_message>
old revisions that didn't get pushed
</commit_message>
<xml_diff>
--- a/Labs/Lab9/Assignment9Rubric-DomainModel-UML-Scaffolding.xlsx
+++ b/Labs/Lab9/Assignment9Rubric-DomainModel-UML-Scaffolding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS246-CourseMaterials\Labs\Lab9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CS246-Repos\CS246-CourseMaterials\Labs\Lab9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676C8EF9-9E45-4F3B-AD5B-B8C76718D01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9726B446-DCE4-4013-950C-791985BA7486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16212" yWindow="5676" windowWidth="15468" windowHeight="10992" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
+    <workbookView xWindow="13272" yWindow="2484" windowWidth="17028" windowHeight="14244" activeTab="1" xr2:uid="{2ED55EEA-81A7-FF44-BCE3-68AB9ADB8259}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -199,8 +199,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EF6DB9-5046-F545-B378-AB8AF91CAAF1}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E21"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -737,10 +743,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+    <row r="3" spans="1:6" s="13" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -777,7 +786,7 @@
       <c r="C6" s="2">
         <v>20</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="10">
         <f>C6/B6</f>
         <v>1</v>
@@ -793,7 +802,7 @@
       <c r="C7" s="2">
         <v>10</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="10">
         <f>C7/B7</f>
         <v>1</v>
@@ -809,7 +818,7 @@
       <c r="C8" s="2">
         <v>10</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="10">
         <f>C8/B8</f>
         <v>1</v>
@@ -827,7 +836,7 @@
         <f>SUM(C6:C8)</f>
         <v>40</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="10">
         <f>C9/B9</f>
         <v>1</v>
@@ -837,7 +846,7 @@
       <c r="A10" s="4"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -846,7 +855,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -859,7 +868,7 @@
       <c r="C12" s="2">
         <v>20</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="10">
         <f>C12/B12</f>
         <v>1</v>
@@ -875,7 +884,7 @@
       <c r="C13" s="2">
         <v>10</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="10">
         <f>C13/B13</f>
         <v>1</v>
@@ -893,7 +902,7 @@
         <f>SUM(C12:C13)</f>
         <v>30</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="10">
         <f>C14/B14</f>
         <v>1</v>
@@ -903,7 +912,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="E15" s="11"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -912,7 +921,7 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -925,7 +934,7 @@
       <c r="C17" s="2">
         <v>15</v>
       </c>
-      <c r="E17" s="11"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="10">
         <f>C17/B17</f>
         <v>1</v>
@@ -941,7 +950,7 @@
       <c r="C18" s="2">
         <v>15</v>
       </c>
-      <c r="E18" s="11"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="10">
         <f>C18/B18</f>
         <v>1</v>
@@ -959,7 +968,7 @@
         <f>SUM(C17:C18)</f>
         <v>30</v>
       </c>
-      <c r="E19" s="11"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="10">
         <f>C19/B19</f>
         <v>1</v>
@@ -969,7 +978,7 @@
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="E20" s="11"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
@@ -983,9 +992,12 @@
         <f>SUM(C9,C14,C19)</f>
         <v>100</v>
       </c>
-      <c r="E21" s="11"/>
+      <c r="E21" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:F3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>